<commit_message>
some new features added
</commit_message>
<xml_diff>
--- a/TestData/FacebookLogin.xlsx
+++ b/TestData/FacebookLogin.xlsx
@@ -22,23 +22,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
+    <t>Usernames</t>
+  </si>
+  <si>
     <t>Jenny Joseph</t>
   </si>
-  <si>
-    <t>Usernames</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,8 +66,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,26 +354,27 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -375,7 +384,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>